<commit_message>
Results from September 22, 2020 run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-09-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-09-22.xlsx
@@ -457,25 +457,25 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C2" t="n">
-        <v>275735</v>
+        <v>277266</v>
       </c>
       <c r="D2" t="n">
-        <v>8457</v>
+        <v>8486</v>
       </c>
       <c r="E2" t="n">
-        <v>38217</v>
+        <v>38467</v>
       </c>
       <c r="F2" t="n">
-        <v>2199</v>
+        <v>2200</v>
       </c>
       <c r="G2" t="n">
-        <v>13.86</v>
+        <v>13.87</v>
       </c>
       <c r="H2" t="n">
-        <v>26</v>
+        <v>25.93</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -507,10 +507,10 @@
         <v>44090</v>
       </c>
       <c r="C3" t="n">
-        <v>161462</v>
+        <v>162214</v>
       </c>
       <c r="D3" t="n">
-        <v>5207</v>
+        <v>5218</v>
       </c>
       <c r="E3" t="n">
         <v>58240</v>
@@ -555,25 +555,25 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44094</v>
+        <v>44096</v>
       </c>
       <c r="C4" t="n">
-        <v>82548</v>
+        <v>83193</v>
       </c>
       <c r="D4" t="n">
-        <v>2037</v>
+        <v>2070</v>
       </c>
       <c r="E4" t="n">
-        <v>3360</v>
+        <v>3412</v>
       </c>
       <c r="F4" t="n">
         <v>68</v>
       </c>
       <c r="G4" t="n">
-        <v>5.91</v>
+        <v>5.93</v>
       </c>
       <c r="H4" t="n">
-        <v>3.38</v>
+        <v>3.34</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -582,10 +582,10 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>56830</v>
+        <v>57492</v>
       </c>
       <c r="L4" t="n">
-        <v>2012</v>
+        <v>2036</v>
       </c>
       <c r="M4" t="n">
         <v>269854</v>
@@ -701,26 +701,26 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>235969</t>
+          <t>236253</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>19152</t>
+          <t>19153</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>36985</v>
+        <v>37018</v>
       </c>
       <c r="F8" t="n">
-        <v>5342</v>
+        <v>5343</v>
       </c>
       <c r="G8" t="n">
-        <v>28.27</v>
+        <v>28.21</v>
       </c>
       <c r="H8" t="n">
         <v>30.42</v>
@@ -732,7 +732,7 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>130838</v>
+        <v>131200</v>
       </c>
       <c r="L8" t="n">
         <v>17562</v>
@@ -807,25 +807,25 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C10" t="n">
-        <v>26900</v>
+        <v>27124</v>
       </c>
       <c r="D10" t="n">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E10" t="n">
-        <v>6742</v>
+        <v>6775</v>
       </c>
       <c r="F10" t="n">
         <v>154</v>
       </c>
       <c r="G10" t="n">
-        <v>26.73</v>
+        <v>26.62</v>
       </c>
       <c r="H10" t="n">
-        <v>36.41</v>
+        <v>36.32</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -834,10 +834,10 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>25222</v>
+        <v>25449</v>
       </c>
       <c r="L10" t="n">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="M10" t="n">
         <v>252321</v>
@@ -971,25 +971,25 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C14" t="n">
-        <v>184409</v>
+        <v>185148</v>
       </c>
       <c r="D14" t="n">
-        <v>2233</v>
+        <v>2261</v>
       </c>
       <c r="E14" t="n">
-        <v>33954</v>
+        <v>34086</v>
       </c>
       <c r="F14" t="n">
-        <v>611</v>
+        <v>622</v>
       </c>
       <c r="G14" t="n">
         <v>18.41</v>
       </c>
       <c r="H14" t="n">
-        <v>27.36</v>
+        <v>27.51</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -1018,20 +1018,20 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C15" t="n">
-        <v>5106</v>
+        <v>5146</v>
       </c>
       <c r="D15" t="n">
         <v>140</v>
       </c>
       <c r="E15" t="n">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
-        <v>20.76</v>
+        <v>20.64</v>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="b">
@@ -1041,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>4649</v>
+        <v>4680</v>
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
@@ -1096,25 +1096,25 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C17" t="n">
-        <v>131405</v>
+        <v>131988</v>
       </c>
       <c r="D17" t="n">
-        <v>2292</v>
+        <v>2304</v>
       </c>
       <c r="E17" t="n">
-        <v>32839</v>
+        <v>33000</v>
       </c>
       <c r="F17" t="n">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="G17" t="n">
-        <v>37.57</v>
+        <v>37.46</v>
       </c>
       <c r="H17" t="n">
-        <v>40.82</v>
+        <v>40.79</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
@@ -1123,10 +1123,10 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>87409</v>
+        <v>88083</v>
       </c>
       <c r="L17" t="n">
-        <v>2212</v>
+        <v>2221</v>
       </c>
       <c r="M17" t="n">
         <v>1293186</v>
@@ -1227,25 +1227,25 @@
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44094</v>
+        <v>44095</v>
       </c>
       <c r="C20" t="n">
-        <v>53692</v>
+        <v>53814</v>
       </c>
       <c r="D20" t="n">
-        <v>3600</v>
+        <v>3601</v>
       </c>
       <c r="E20" t="n">
-        <v>7331</v>
+        <v>7333</v>
       </c>
       <c r="F20" t="n">
         <v>662</v>
       </c>
       <c r="G20" t="n">
-        <v>13.65</v>
+        <v>13.63</v>
       </c>
       <c r="H20" t="n">
-        <v>18.39</v>
+        <v>18.38</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
@@ -1274,25 +1274,25 @@
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C21" t="n">
-        <v>117325</v>
+        <v>117828</v>
       </c>
       <c r="D21" t="n">
-        <v>6604</v>
+        <v>6616</v>
       </c>
       <c r="E21" t="n">
-        <v>25700</v>
+        <v>25758</v>
       </c>
       <c r="F21" t="n">
-        <v>2530</v>
+        <v>2531</v>
       </c>
       <c r="G21" t="n">
-        <v>21.9</v>
+        <v>21.86</v>
       </c>
       <c r="H21" t="n">
-        <v>38.31</v>
+        <v>38.26</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
@@ -1409,7 +1409,7 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>An error occurred. ... ValueError("invalid literal for int() with base 10: '10,429'")</t>
+          <t>An error occurred. ... ValueError("invalid literal for int() with base 10: '10,700'")</t>
         </is>
       </c>
     </row>
@@ -1453,22 +1453,22 @@
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C26" t="n">
-        <v>4191</v>
+        <v>4316</v>
       </c>
       <c r="D26" t="n">
         <v>44</v>
       </c>
       <c r="E26" t="n">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="F26" t="n">
         <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>5.91</v>
+        <v>5.87</v>
       </c>
       <c r="H26" t="n">
         <v>2.33</v>
@@ -1480,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>3806</v>
+        <v>3954</v>
       </c>
       <c r="L26" t="n">
         <v>43</v>
@@ -1533,16 +1533,16 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C28" t="n">
-        <v>127796</v>
+        <v>127969</v>
       </c>
       <c r="D28" t="n">
-        <v>9317</v>
+        <v>9328</v>
       </c>
       <c r="E28" t="n">
-        <v>12119</v>
+        <v>12136</v>
       </c>
       <c r="F28" t="n">
         <v>759</v>
@@ -1551,7 +1551,7 @@
         <v>9.48</v>
       </c>
       <c r="H28" t="n">
-        <v>8.15</v>
+        <v>8.140000000000001</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -1580,20 +1580,20 @@
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C29" t="n">
-        <v>167153</v>
+        <v>167515</v>
       </c>
       <c r="D29" t="n">
-        <v>3055</v>
+        <v>3085</v>
       </c>
       <c r="E29" t="n">
-        <v>14740</v>
+        <v>14783</v>
       </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
-        <v>14.21</v>
+        <v>14.2</v>
       </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="b">
@@ -1603,7 +1603,7 @@
         <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>103726</v>
+        <v>104100</v>
       </c>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="n">
@@ -1625,20 +1625,20 @@
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C30" t="n">
-        <v>39056</v>
+        <v>39232</v>
       </c>
       <c r="D30" t="n">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E30" t="n">
-        <v>5844</v>
+        <v>5916</v>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="n">
-        <v>23.2</v>
+        <v>23.19</v>
       </c>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="b">
@@ -1648,7 +1648,7 @@
         <v>1</v>
       </c>
       <c r="K30" t="n">
-        <v>25195</v>
+        <v>25508</v>
       </c>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="n">
@@ -1703,25 +1703,25 @@
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C32" t="n">
-        <v>114262</v>
+        <v>115319</v>
       </c>
       <c r="D32" t="n">
-        <v>1807</v>
+        <v>1864</v>
       </c>
       <c r="E32" t="n">
-        <v>11637</v>
+        <v>11638</v>
       </c>
       <c r="F32" t="n">
-        <v>476</v>
+        <v>488</v>
       </c>
       <c r="G32" t="n">
         <v>26.33</v>
       </c>
       <c r="H32" t="n">
-        <v>31.59</v>
+        <v>32.02</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
@@ -1730,10 +1730,10 @@
         <v>1</v>
       </c>
       <c r="K32" t="n">
-        <v>44197</v>
+        <v>44196</v>
       </c>
       <c r="L32" t="n">
-        <v>1507</v>
+        <v>1524</v>
       </c>
       <c r="M32" t="n">
         <v>704896</v>
@@ -1754,21 +1754,21 @@
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>64394</t>
+          <t>65044</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>441</t>
+          <t>443</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1355</t>
+          <t>1366</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1780,7 +1780,7 @@
         <v>2.1</v>
       </c>
       <c r="H33" t="n">
-        <v>1.59</v>
+        <v>1.58</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
@@ -1809,25 +1809,25 @@
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>44094</v>
+        <v>44095</v>
       </c>
       <c r="C34" t="n">
-        <v>93556</v>
+        <v>94021</v>
       </c>
       <c r="D34" t="n">
-        <v>2810</v>
+        <v>2846</v>
       </c>
       <c r="E34" t="n">
-        <v>37153</v>
+        <v>37272</v>
       </c>
       <c r="F34" t="n">
-        <v>1311</v>
+        <v>1322</v>
       </c>
       <c r="G34" t="n">
-        <v>39.71</v>
+        <v>39.64</v>
       </c>
       <c r="H34" t="n">
-        <v>46.65</v>
+        <v>46.45</v>
       </c>
       <c r="I34" t="b">
         <v>1</v>
@@ -1907,25 +1907,25 @@
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C36" t="n">
-        <v>90942</v>
+        <v>91422</v>
       </c>
       <c r="D36" t="n">
-        <v>1969</v>
+        <v>1979</v>
       </c>
       <c r="E36" t="n">
-        <v>16342</v>
+        <v>16382</v>
       </c>
       <c r="F36" t="n">
         <v>189</v>
       </c>
       <c r="G36" t="n">
-        <v>17.97</v>
+        <v>17.92</v>
       </c>
       <c r="H36" t="n">
-        <v>9.6</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="I36" t="b">
         <v>1</v>
@@ -1986,15 +1986,29 @@
           <t>Texas</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
+      <c r="B38" s="2" t="n">
+        <v>44096</v>
+      </c>
+      <c r="C38" t="n">
+        <v>52768</v>
+      </c>
+      <c r="D38" t="n">
+        <v>14994</v>
+      </c>
+      <c r="E38" t="n">
+        <v>8716</v>
+      </c>
+      <c r="F38" t="n">
+        <v>1704</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.11</v>
+      </c>
       <c r="I38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="b">
         <v>0</v>
@@ -2009,7 +2023,7 @@
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>An error occurred. ... KeyError("None of ['Race/Ethnicity'] are in the columns")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -2053,25 +2067,25 @@
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C40" t="n">
-        <v>41388</v>
+        <v>41785</v>
       </c>
       <c r="D40" t="n">
-        <v>452</v>
+        <v>461</v>
       </c>
       <c r="E40" t="n">
-        <v>2251</v>
+        <v>2257</v>
       </c>
       <c r="F40" t="n">
         <v>33</v>
       </c>
       <c r="G40" t="n">
-        <v>7.04</v>
+        <v>7.03</v>
       </c>
       <c r="H40" t="n">
-        <v>7.88</v>
+        <v>7.71</v>
       </c>
       <c r="I40" t="b">
         <v>0</v>
@@ -2080,10 +2094,10 @@
         <v>1</v>
       </c>
       <c r="K40" t="n">
-        <v>31995</v>
+        <v>32113</v>
       </c>
       <c r="L40" t="n">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="M40" t="n">
         <v>90860</v>
@@ -2104,19 +2118,19 @@
         </is>
       </c>
       <c r="B41" s="3" t="n">
-        <v>44094</v>
+        <v>44095</v>
       </c>
       <c r="C41" t="n">
-        <v>781694</v>
+        <v>784324</v>
       </c>
       <c r="D41" t="n">
-        <v>15018</v>
+        <v>15071</v>
       </c>
       <c r="E41" t="n">
-        <v>23014</v>
+        <v>23073</v>
       </c>
       <c r="F41" t="n">
-        <v>1138</v>
+        <v>1140</v>
       </c>
       <c r="G41" t="n">
         <v>4.26</v>
@@ -2131,10 +2145,10 @@
         <v>0</v>
       </c>
       <c r="K41" t="n">
-        <v>539935</v>
+        <v>541492</v>
       </c>
       <c r="L41" t="n">
-        <v>14695</v>
+        <v>14723</v>
       </c>
       <c r="M41" t="n">
         <v>2267875</v>
@@ -2184,10 +2198,10 @@
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C43" t="n">
-        <v>1719</v>
+        <v>1721</v>
       </c>
       <c r="D43" t="n">
         <v>58</v>
@@ -2199,7 +2213,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>10.46</v>
+        <v>10.45</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -2211,7 +2225,7 @@
         <v>1</v>
       </c>
       <c r="K43" t="n">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="L43" t="n">
         <v>58</v>
@@ -2235,20 +2249,20 @@
         </is>
       </c>
       <c r="B44" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C44" t="n">
-        <v>27683</v>
+        <v>27790</v>
       </c>
       <c r="D44" t="n">
-        <v>851</v>
+        <v>854</v>
       </c>
       <c r="E44" t="n">
         <v>495</v>
       </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="n">
-        <v>1.79</v>
+        <v>1.78</v>
       </c>
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="b">
@@ -2278,25 +2292,25 @@
         </is>
       </c>
       <c r="B45" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C45" t="n">
-        <v>677362</v>
+        <v>679776</v>
       </c>
       <c r="D45" t="n">
-        <v>13317</v>
+        <v>13416</v>
       </c>
       <c r="E45" t="n">
-        <v>90985</v>
+        <v>91438</v>
       </c>
       <c r="F45" t="n">
-        <v>2336</v>
+        <v>2354</v>
       </c>
       <c r="G45" t="n">
-        <v>13.43</v>
+        <v>13.45</v>
       </c>
       <c r="H45" t="n">
-        <v>17.54</v>
+        <v>17.55</v>
       </c>
       <c r="I45" t="b">
         <v>1</v>
@@ -2401,25 +2415,25 @@
         </is>
       </c>
       <c r="B48" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C48" t="n">
-        <v>65399</v>
+        <v>66053</v>
       </c>
       <c r="D48" t="n">
-        <v>2018</v>
+        <v>2025</v>
       </c>
       <c r="E48" t="n">
-        <v>2871</v>
+        <v>2873</v>
       </c>
       <c r="F48" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G48" t="n">
-        <v>5.23</v>
+        <v>5.21</v>
       </c>
       <c r="H48" t="n">
-        <v>6.46</v>
+        <v>6.49</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
@@ -2428,10 +2442,10 @@
         <v>0</v>
       </c>
       <c r="K48" t="n">
-        <v>54863</v>
+        <v>55181</v>
       </c>
       <c r="L48" t="n">
-        <v>1981</v>
+        <v>1987</v>
       </c>
       <c r="M48" t="n">
         <v>227938</v>
@@ -2452,25 +2466,25 @@
         </is>
       </c>
       <c r="B49" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C49" t="n">
-        <v>44925</v>
+        <v>45147</v>
       </c>
       <c r="D49" t="n">
-        <v>760</v>
+        <v>765</v>
       </c>
       <c r="E49" t="n">
-        <v>1665</v>
+        <v>1670</v>
       </c>
       <c r="F49" t="n">
         <v>32</v>
       </c>
       <c r="G49" t="n">
-        <v>4.49</v>
+        <v>4.48</v>
       </c>
       <c r="H49" t="n">
-        <v>4.27</v>
+        <v>4.24</v>
       </c>
       <c r="I49" t="b">
         <v>0</v>
@@ -2479,10 +2493,10 @@
         <v>0</v>
       </c>
       <c r="K49" t="n">
-        <v>37042</v>
+        <v>37262</v>
       </c>
       <c r="L49" t="n">
-        <v>750</v>
+        <v>755</v>
       </c>
       <c r="M49" t="n">
         <v>166412</v>
@@ -2536,22 +2550,22 @@
         </is>
       </c>
       <c r="B51" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C51" t="n">
-        <v>146281</v>
+        <v>147070</v>
       </c>
       <c r="D51" t="n">
-        <v>8004</v>
+        <v>8023</v>
       </c>
       <c r="E51" t="n">
-        <v>19841</v>
+        <v>19973</v>
       </c>
       <c r="F51" t="n">
         <v>1651</v>
       </c>
       <c r="G51" t="n">
-        <v>25.75</v>
+        <v>25.68</v>
       </c>
       <c r="H51" t="n">
         <v>20.81</v>
@@ -2563,7 +2577,7 @@
         <v>1</v>
       </c>
       <c r="K51" t="n">
-        <v>77055</v>
+        <v>77780</v>
       </c>
       <c r="L51" t="n">
         <v>7934</v>
@@ -2620,25 +2634,25 @@
         </is>
       </c>
       <c r="B53" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C53" t="n">
-        <v>307339</v>
+        <v>308221</v>
       </c>
       <c r="D53" t="n">
-        <v>6604</v>
+        <v>6677</v>
       </c>
       <c r="E53" t="n">
-        <v>79483</v>
+        <v>80047</v>
       </c>
       <c r="F53" t="n">
-        <v>2743</v>
+        <v>2774</v>
       </c>
       <c r="G53" t="n">
-        <v>25.86</v>
+        <v>25.97</v>
       </c>
       <c r="H53" t="n">
-        <v>41.54</v>
+        <v>41.55</v>
       </c>
       <c r="I53" t="b">
         <v>1</v>
@@ -2743,25 +2757,25 @@
         </is>
       </c>
       <c r="B56" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C56" t="n">
-        <v>112027</v>
+        <v>112626</v>
       </c>
       <c r="D56" t="n">
-        <v>3287</v>
+        <v>3295</v>
       </c>
       <c r="E56" t="n">
-        <v>10959</v>
+        <v>11005</v>
       </c>
       <c r="F56" t="n">
         <v>444</v>
       </c>
       <c r="G56" t="n">
-        <v>9.779999999999999</v>
+        <v>9.77</v>
       </c>
       <c r="H56" t="n">
-        <v>13.51</v>
+        <v>13.47</v>
       </c>
       <c r="I56" t="b">
         <v>1</v>
@@ -2823,25 +2837,25 @@
         </is>
       </c>
       <c r="B58" s="2" t="n">
-        <v>44095</v>
+        <v>44096</v>
       </c>
       <c r="C58" t="n">
-        <v>61917</v>
+        <v>62731</v>
       </c>
       <c r="D58" t="n">
-        <v>1112</v>
+        <v>1119</v>
       </c>
       <c r="E58" t="n">
-        <v>4890</v>
+        <v>4962</v>
       </c>
       <c r="F58" t="n">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G58" t="n">
-        <v>11.52</v>
+        <v>11.66</v>
       </c>
       <c r="H58" t="n">
-        <v>12.91</v>
+        <v>12.93</v>
       </c>
       <c r="I58" t="b">
         <v>0</v>
@@ -2850,10 +2864,10 @@
         <v>1</v>
       </c>
       <c r="K58" t="n">
-        <v>42456</v>
+        <v>42562</v>
       </c>
       <c r="L58" t="n">
-        <v>1015</v>
+        <v>1020</v>
       </c>
       <c r="M58" t="n">
         <v>354112</v>
@@ -2874,25 +2888,25 @@
         </is>
       </c>
       <c r="B59" s="2" t="n">
-        <v>44094</v>
+        <v>44095</v>
       </c>
       <c r="C59" t="n">
-        <v>261446</v>
+        <v>262133</v>
       </c>
       <c r="D59" t="n">
-        <v>6366</v>
+        <v>6401</v>
       </c>
       <c r="E59" t="n">
-        <v>7512</v>
+        <v>7545</v>
       </c>
       <c r="F59" t="n">
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="G59" t="n">
-        <v>4.8</v>
+        <v>4.81</v>
       </c>
       <c r="H59" t="n">
-        <v>9.779999999999999</v>
+        <v>9.81</v>
       </c>
       <c r="I59" t="b">
         <v>0</v>
@@ -2901,10 +2915,10 @@
         <v>0</v>
       </c>
       <c r="K59" t="n">
-        <v>156406</v>
+        <v>156893</v>
       </c>
       <c r="L59" t="n">
-        <v>5989</v>
+        <v>6022</v>
       </c>
       <c r="M59" t="n">
         <v>823987</v>

</xml_diff>